<commit_message>
changed in excel file
</commit_message>
<xml_diff>
--- a/testData/OpenCart_LoginData.xlsx
+++ b/testData/OpenCart_LoginData.xlsx
@@ -35,7 +35,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>Exp Res</t>
+    <t>Exp Result</t>
   </si>
   <si>
     <t>bhaskar@gmail.com</t>
@@ -711,7 +711,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,13 +1061,14 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="36.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="11.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
changed the logic based on tittle to based pagetextheader
</commit_message>
<xml_diff>
--- a/testData/OpenCart_LoginData.xlsx
+++ b/testData/OpenCart_LoginData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -38,15 +39,18 @@
     <t>Exp Result</t>
   </si>
   <si>
-    <t>bhaskar@gmail.com</t>
-  </si>
-  <si>
-    <t>test123</t>
+    <t>bhaskar4@gmail.com</t>
+  </si>
+  <si>
+    <t>Test123</t>
   </si>
   <si>
     <t>Valid</t>
   </si>
   <si>
+    <t>Test1234</t>
+  </si>
+  <si>
     <t>InValid</t>
   </si>
   <si>
@@ -56,19 +60,19 @@
     <t>Bhaskar@123</t>
   </si>
   <si>
+    <t>Bhaskar@1234</t>
+  </si>
+  <si>
     <t>Invalid</t>
   </si>
   <si>
-    <t>bhaskar1@gmail.com</t>
-  </si>
-  <si>
-    <t>test12345</t>
-  </si>
-  <si>
-    <t>bhaskar2@gmail.com</t>
-  </si>
-  <si>
-    <t>test1234</t>
+    <t>bhaskar3@gmail.com</t>
+  </si>
+  <si>
+    <t>Test12345</t>
+  </si>
+  <si>
+    <t>Test123456</t>
   </si>
 </sst>
 </file>
@@ -90,6 +94,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,14 +113,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -575,10 +579,10 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -707,11 +711,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,13 +1062,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B8" sqref="C2 B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="36.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1072,18 +1076,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1094,22 +1098,22 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1117,67 +1121,117 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>10</v>
+      <c r="A6" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>10</v>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="bhaskar@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId1" display="bhaskar@gmail.com"/>
-    <hyperlink ref="A8" r:id="rId2" display="bhaskar2@gmail.com"/>
-    <hyperlink ref="A9" r:id="rId2" display="bhaskar2@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="bhaskar4@gmail.com" tooltip="mailto:bhaskar4@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId1" display="bhaskar4@gmail.com" tooltip="mailto:bhaskar4@gmail.com"/>
+    <hyperlink ref="A6" r:id="rId2" display="bhaskar3@gmail.com"/>
+    <hyperlink ref="A7" r:id="rId2" display="bhaskar3@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId3" display="Bhaskar@1234"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="28.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="31.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="25.4444444444444" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="bhaskar3@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId1" display="bhaskar3@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Bhaskar@1234"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed Null Pointer Exception that causes empty data
</commit_message>
<xml_diff>
--- a/testData/OpenCart_LoginData.xlsx
+++ b/testData/OpenCart_LoginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Test123456</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -1062,13 +1068,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="36.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1149,6 +1155,22 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Docker-compose.yaml file  and moved pageobject to src/main/java
</commit_message>
<xml_diff>
--- a/testData/OpenCart_LoginData.xlsx
+++ b/testData/OpenCart_LoginData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Username</t>
   </si>
@@ -54,6 +54,18 @@
     <t>InValid</t>
   </si>
   <si>
+    <t>bhaskar3@gmail.com</t>
+  </si>
+  <si>
+    <t>Test12345</t>
+  </si>
+  <si>
+    <t>Test123456</t>
+  </si>
+  <si>
+    <t>bhaskar</t>
+  </si>
+  <si>
     <t>Bhaskarpattepu105@gmail.com</t>
   </si>
   <si>
@@ -64,21 +76,6 @@
   </si>
   <si>
     <t>Invalid</t>
-  </si>
-  <si>
-    <t>bhaskar3@gmail.com</t>
-  </si>
-  <si>
-    <t>Test12345</t>
-  </si>
-  <si>
-    <t>Test123456</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
 </sst>
 </file>
@@ -1068,13 +1065,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="36.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1115,7 +1112,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -1126,51 +1123,22 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6"/>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1178,9 +1146,8 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="bhaskar4@gmail.com" tooltip="mailto:bhaskar4@gmail.com"/>
     <hyperlink ref="A3" r:id="rId1" display="bhaskar4@gmail.com" tooltip="mailto:bhaskar4@gmail.com"/>
-    <hyperlink ref="A6" r:id="rId2" display="bhaskar3@gmail.com"/>
-    <hyperlink ref="A7" r:id="rId2" display="bhaskar3@gmail.com"/>
-    <hyperlink ref="B5" r:id="rId3" display="Bhaskar@1234"/>
+    <hyperlink ref="A4" r:id="rId2" display="bhaskar3@gmail.com"/>
+    <hyperlink ref="A5" r:id="rId2" display="bhaskar3@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1205,10 +1172,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1216,21 +1183,21 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1238,10 +1205,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
changed name of testname in report
</commit_message>
<xml_diff>
--- a/testData/OpenCart_LoginData.xlsx
+++ b/testData/OpenCart_LoginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="9887" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1068,7 +1068,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -1112,7 +1112,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">

</xml_diff>